<commit_message>
ajout du flux vidéo et squelettes des fichiers
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
   <si>
     <t>Jour</t>
   </si>
@@ -91,16 +91,10 @@
     <t>Lecture du cahier des charges</t>
   </si>
   <si>
-    <t>1h</t>
-  </si>
-  <si>
     <t>Entretien avec M.Bonvin</t>
   </si>
   <si>
     <t>Planification</t>
-  </si>
-  <si>
-    <t>0,5h</t>
   </si>
   <si>
     <t>Le planning avait été estimé par M. Bonvin</t>
@@ -116,25 +110,37 @@
 Mouvement de caméra oui ou non / Maquette de la page de streaming</t>
   </si>
   <si>
-    <t>1,5h</t>
-  </si>
-  <si>
     <t>Installation Apache et PHP sur AlphaBot2</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
     <t>Diagramme de classes</t>
   </si>
   <si>
     <t>Total 07.mai</t>
   </si>
   <si>
-    <t>8h</t>
-  </si>
-  <si>
     <t>Pas fini</t>
+  </si>
+  <si>
+    <t>Maquette</t>
+  </si>
+  <si>
+    <t>Diagramme fini</t>
+  </si>
+  <si>
+    <t>Installation des librairies</t>
+  </si>
+  <si>
+    <t>Les librairies sur le raspberry pi sont installés en parralèlle, je ne les comptes pas dans le temps</t>
+  </si>
+  <si>
+    <t>Mise en place du squelette du programme</t>
+  </si>
+  <si>
+    <t>Selon diagramme de classes effectué</t>
+  </si>
+  <si>
+    <t>Gestion du flux sur une page web</t>
   </si>
 </sst>
 </file>
@@ -452,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -500,11 +506,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -512,17 +515,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,23 +539,23 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -562,13 +571,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D52" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
-  <autoFilter ref="A1:D52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D53" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:D53"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Date" dataDxfId="5"/>
     <tableColumn id="2" name="Tâche" dataDxfId="4"/>
-    <tableColumn id="3" name="Temps H" dataDxfId="0"/>
-    <tableColumn id="4" name="Commentaire" dataDxfId="3"/>
+    <tableColumn id="3" name="Temps H" dataDxfId="3"/>
+    <tableColumn id="4" name="Commentaire" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -873,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AB7" sqref="AB7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,50 +898,50 @@
       <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="35">
         <v>1</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35">
+      <c r="D3" s="34"/>
+      <c r="E3" s="34">
         <v>2</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35">
+      <c r="F3" s="34"/>
+      <c r="G3" s="34">
         <v>3</v>
       </c>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35">
+      <c r="H3" s="34"/>
+      <c r="I3" s="34">
         <v>4</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34">
         <v>5</v>
       </c>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35">
+      <c r="L3" s="34"/>
+      <c r="M3" s="34">
         <v>6</v>
       </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35">
+      <c r="N3" s="34"/>
+      <c r="O3" s="34">
         <v>7</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35">
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34">
         <v>8</v>
       </c>
-      <c r="R3" s="35"/>
-      <c r="S3" s="35">
+      <c r="R3" s="34"/>
+      <c r="S3" s="34">
         <v>9</v>
       </c>
-      <c r="T3" s="35"/>
-      <c r="U3" s="35">
+      <c r="T3" s="34"/>
+      <c r="U3" s="34">
         <v>10</v>
       </c>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35">
+      <c r="V3" s="34"/>
+      <c r="W3" s="34">
         <v>11</v>
       </c>
-      <c r="X3" s="35"/>
+      <c r="X3" s="34"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
@@ -1329,17 +1338,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1351,7 +1360,7 @@
   <dimension ref="B1:X15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1365,50 +1374,50 @@
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="35">
         <v>1</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34">
         <v>2</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35">
+      <c r="F2" s="34"/>
+      <c r="G2" s="34">
         <v>3</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35">
+      <c r="H2" s="34"/>
+      <c r="I2" s="34">
         <v>4</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35">
+      <c r="J2" s="34"/>
+      <c r="K2" s="34">
         <v>5</v>
       </c>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35">
+      <c r="L2" s="34"/>
+      <c r="M2" s="34">
         <v>6</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35">
+      <c r="N2" s="34"/>
+      <c r="O2" s="34">
         <v>7</v>
       </c>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35">
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34">
         <v>8</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="35">
+      <c r="R2" s="34"/>
+      <c r="S2" s="34">
         <v>9</v>
       </c>
-      <c r="T2" s="35"/>
-      <c r="U2" s="35">
+      <c r="T2" s="34"/>
+      <c r="U2" s="34">
         <v>10</v>
       </c>
-      <c r="V2" s="35"/>
-      <c r="W2" s="35">
+      <c r="V2" s="34"/>
+      <c r="W2" s="34">
         <v>11</v>
       </c>
-      <c r="X2" s="35"/>
+      <c r="X2" s="34"/>
     </row>
     <row r="3" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
@@ -1487,7 +1496,7 @@
       </c>
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="25"/>
@@ -1514,7 +1523,7 @@
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="29"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
@@ -1541,7 +1550,7 @@
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
+      <c r="E6" s="24"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
@@ -1703,7 +1712,7 @@
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
-      <c r="E12" s="28"/>
+      <c r="E12" s="24"/>
       <c r="F12" s="28"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
@@ -1784,7 +1793,7 @@
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
-      <c r="E15" s="31"/>
+      <c r="E15" s="24"/>
       <c r="F15" s="31"/>
       <c r="G15" s="31"/>
       <c r="H15" s="31"/>
@@ -1807,17 +1816,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1826,139 +1835,216 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="40"/>
-    <col min="4" max="4" width="62.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="6.77734375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="34.5546875" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" style="37"/>
+    <col min="4" max="4" width="62.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="33" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="34">
+      <c r="K1" s="38"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="39">
         <v>43592</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="40">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="39">
+        <v>43592</v>
+      </c>
+      <c r="B3" s="33" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="34">
+      <c r="C3" s="41">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="39">
         <v>43592</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="34">
+      <c r="C4" s="40">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D4" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="39">
         <v>43592</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="37" t="s">
+      <c r="B5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C5" s="41">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="39">
+        <v>43592</v>
+      </c>
+      <c r="B6" s="33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="34">
+      <c r="C6" s="40">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="39">
         <v>43592</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="34">
+      <c r="B7" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="41">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="39">
         <v>43592</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="37" t="s">
+      <c r="B8" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="40">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="39">
+        <v>43592</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="41">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="39">
+        <v>43592</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="36">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="39"/>
+      <c r="B11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="C11" s="36">
+        <f>SUM(C2:C10)</f>
+        <v>0.33333333333333337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="39">
+        <v>43593</v>
+      </c>
+      <c r="B12" s="33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="34">
-        <v>43592</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="38" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="34">
-        <v>43592</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C12" s="36">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="39">
+        <v>43593</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="36">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="39">
+        <v>43593</v>
+      </c>
+      <c r="B14" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="34">
-        <v>43592</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C14" s="36">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="39">
+        <v>43593</v>
+      </c>
+      <c r="B15" s="33" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="34"/>
-      <c r="B10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>32</v>
+      <c r="C15" s="36">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="39">
+        <v>43593</v>
+      </c>
+      <c r="B16" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="36">
+        <v>6.25E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Possible de dessiner sur le stream vidéo
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Jour</t>
   </si>
@@ -141,6 +141,13 @@
   </si>
   <si>
     <t>Gestion du flux sur une page web</t>
+  </si>
+  <si>
+    <t>Difficulté à ajouter le carré vert (position aléatoire)
+Finalement réussi</t>
+  </si>
+  <si>
+    <t>Total 08.mai</t>
   </si>
 </sst>
 </file>
@@ -509,12 +516,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -533,6 +534,12 @@
     <xf numFmtId="20" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,13 +549,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -571,13 +578,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D53" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D53" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D53"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Date" dataDxfId="5"/>
-    <tableColumn id="2" name="Tâche" dataDxfId="4"/>
-    <tableColumn id="3" name="Temps H" dataDxfId="3"/>
-    <tableColumn id="4" name="Commentaire" dataDxfId="2"/>
+    <tableColumn id="1" name="Date" dataDxfId="3"/>
+    <tableColumn id="2" name="Tâche" dataDxfId="2"/>
+    <tableColumn id="3" name="Temps H" dataDxfId="1"/>
+    <tableColumn id="4" name="Commentaire" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -882,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,50 +905,50 @@
       <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="41">
         <v>1</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34">
+      <c r="D3" s="40"/>
+      <c r="E3" s="40">
         <v>2</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34">
+      <c r="F3" s="40"/>
+      <c r="G3" s="40">
         <v>3</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34">
+      <c r="H3" s="40"/>
+      <c r="I3" s="40">
         <v>4</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34">
+      <c r="J3" s="40"/>
+      <c r="K3" s="40">
         <v>5</v>
       </c>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34">
+      <c r="L3" s="40"/>
+      <c r="M3" s="40">
         <v>6</v>
       </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34">
+      <c r="N3" s="40"/>
+      <c r="O3" s="40">
         <v>7</v>
       </c>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34">
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40">
         <v>8</v>
       </c>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34">
+      <c r="R3" s="40"/>
+      <c r="S3" s="40">
         <v>9</v>
       </c>
-      <c r="T3" s="34"/>
-      <c r="U3" s="34">
+      <c r="T3" s="40"/>
+      <c r="U3" s="40">
         <v>10</v>
       </c>
-      <c r="V3" s="34"/>
-      <c r="W3" s="34">
+      <c r="V3" s="40"/>
+      <c r="W3" s="40">
         <v>11</v>
       </c>
-      <c r="X3" s="34"/>
+      <c r="X3" s="40"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
@@ -1338,17 +1345,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1359,8 +1366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1374,50 +1381,50 @@
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="41">
         <v>1</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34">
+      <c r="D2" s="40"/>
+      <c r="E2" s="40">
         <v>2</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34">
+      <c r="F2" s="40"/>
+      <c r="G2" s="40">
         <v>3</v>
       </c>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34">
+      <c r="H2" s="40"/>
+      <c r="I2" s="40">
         <v>4</v>
       </c>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34">
+      <c r="J2" s="40"/>
+      <c r="K2" s="40">
         <v>5</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34">
+      <c r="L2" s="40"/>
+      <c r="M2" s="40">
         <v>6</v>
       </c>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34">
+      <c r="N2" s="40"/>
+      <c r="O2" s="40">
         <v>7</v>
       </c>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34">
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40">
         <v>8</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34">
+      <c r="R2" s="40"/>
+      <c r="S2" s="40">
         <v>9</v>
       </c>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34">
+      <c r="T2" s="40"/>
+      <c r="U2" s="40">
         <v>10</v>
       </c>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34">
+      <c r="V2" s="40"/>
+      <c r="W2" s="40">
         <v>11</v>
       </c>
-      <c r="X2" s="34"/>
+      <c r="X2" s="40"/>
     </row>
     <row r="3" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
@@ -1551,7 +1558,7 @@
       <c r="C6" s="27"/>
       <c r="D6" s="28"/>
       <c r="E6" s="24"/>
-      <c r="F6" s="28"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
       <c r="I6" s="28"/>
@@ -1713,7 +1720,7 @@
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="28"/>
+      <c r="F12" s="24"/>
       <c r="G12" s="28"/>
       <c r="H12" s="28"/>
       <c r="I12" s="28"/>
@@ -1794,7 +1801,7 @@
       <c r="C15" s="24"/>
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
-      <c r="F15" s="31"/>
+      <c r="F15" s="24"/>
       <c r="G15" s="31"/>
       <c r="H15" s="31"/>
       <c r="I15" s="31"/>
@@ -1816,17 +1823,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1835,66 +1842,66 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.77734375" style="33" customWidth="1"/>
     <col min="2" max="2" width="34.5546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="37"/>
+    <col min="3" max="3" width="11.5546875" style="35"/>
     <col min="4" max="4" width="62.6640625" style="33" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="11.5546875" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="34" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="35" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="38"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="39">
+      <c r="A2" s="37">
         <v>43592</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="40">
+      <c r="C2" s="38">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="39">
+      <c r="A3" s="37">
         <v>43592</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="39">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="39">
+      <c r="A4" s="37">
         <v>43592</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="38">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D4" s="33" t="s">
@@ -1902,24 +1909,24 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="39">
+      <c r="A5" s="37">
         <v>43592</v>
       </c>
       <c r="B5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="39">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="39">
+      <c r="A6" s="37">
         <v>43592</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="38">
         <v>6.25E-2</v>
       </c>
       <c r="D6" s="33" t="s">
@@ -1927,46 +1934,46 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="39">
+      <c r="A7" s="37">
         <v>43592</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="39">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="39">
+      <c r="A8" s="37">
         <v>43592</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="38">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="39">
+      <c r="A9" s="37">
         <v>43592</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="41">
+      <c r="C9" s="39">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="39">
+      <c r="A10" s="37">
         <v>43592</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="34">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D10" s="33" t="s">
@@ -1974,23 +1981,23 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
+      <c r="A11" s="37"/>
       <c r="B11" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="34">
         <f>SUM(C2:C10)</f>
         <v>0.33333333333333337</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="39">
+      <c r="A12" s="37">
         <v>43593</v>
       </c>
       <c r="B12" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="34">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D12" s="33" t="s">
@@ -1998,13 +2005,13 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="39">
+      <c r="A13" s="37">
         <v>43593</v>
       </c>
       <c r="B13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="34">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D13" s="33" t="s">
@@ -2012,40 +2019,55 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="39">
+      <c r="A14" s="37">
         <v>43593</v>
       </c>
       <c r="B14" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="36">
-        <v>2.0833333333333332E-2</v>
+      <c r="C14" s="34">
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="39">
+      <c r="A15" s="37">
         <v>43593</v>
       </c>
       <c r="B15" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="36">
-        <v>2.0833333333333332E-2</v>
+      <c r="C15" s="34">
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="39">
+    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="37">
         <v>43593</v>
       </c>
       <c r="B16" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="36">
-        <v>6.25E-2</v>
-      </c>
+      <c r="C16" s="34">
+        <v>0.14583333333333334</v>
+      </c>
+      <c r="D16" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="34">
+        <f>SUM(C12:C16)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C18" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Mise a jour commentaire
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Jour</t>
   </si>
@@ -148,6 +148,29 @@
   </si>
   <si>
     <t>Total 08.mai</t>
+  </si>
+  <si>
+    <t>Test des différents moyen d'analyse</t>
+  </si>
+  <si>
+    <t>OpenCV
+Scikit-image
+Propre algorithme</t>
+  </si>
+  <si>
+    <t>Visite des experts</t>
+  </si>
+  <si>
+    <t>Discuté avec M.Rulo sur l'avancée du projet et mon ressenti</t>
+  </si>
+  <si>
+    <t>Implémentation de la méthode d'analyse avec scikit-image</t>
+  </si>
+  <si>
+    <t>Déplacement du robot en fonction de l'image analysé</t>
+  </si>
+  <si>
+    <t>Total 09.mai</t>
   </si>
 </sst>
 </file>
@@ -889,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1366,8 +1389,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1586,7 +1609,7 @@
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
       <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="28"/>
       <c r="I7" s="28"/>
       <c r="J7" s="28"/>
@@ -1641,7 +1664,7 @@
       <c r="E9" s="28"/>
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
+      <c r="H9" s="24"/>
       <c r="I9" s="28"/>
       <c r="J9" s="28"/>
       <c r="K9" s="28"/>
@@ -1721,8 +1744,8 @@
       <c r="D12" s="24"/>
       <c r="E12" s="24"/>
       <c r="F12" s="24"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
       <c r="I12" s="28"/>
       <c r="J12" s="28"/>
       <c r="K12" s="28"/>
@@ -1802,8 +1825,8 @@
       <c r="D15" s="24"/>
       <c r="E15" s="24"/>
       <c r="F15" s="24"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
       <c r="I15" s="31"/>
       <c r="J15" s="31"/>
       <c r="K15" s="31"/>
@@ -1842,10 +1865,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2057,7 +2080,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" s="33" t="s">
         <v>37</v>
       </c>
@@ -2066,8 +2089,75 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C18" s="34"/>
+    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="37">
+        <v>43594</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="34">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="37">
+        <v>43594</v>
+      </c>
+      <c r="B19" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="34">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="37">
+        <v>43594</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="34">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="37">
+        <v>43594</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="34">
+        <v>0.10416666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="37">
+        <v>43594</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="34">
+        <f>SUM(C18:C22)</f>
+        <v>0.33333333333333337</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Améliration :  - Déplacement  - Analyse d'iamge
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>Jour</t>
   </si>
@@ -186,6 +186,21 @@
   </si>
   <si>
     <t>Permet d'être plus clair sur les différentes utilités des classes/fichiers</t>
+  </si>
+  <si>
+    <t>Meilleure méthode de déplacement du robot</t>
+  </si>
+  <si>
+    <t>Bien plus fluide et précis</t>
+  </si>
+  <si>
+    <t>Analyse d'image plus précise</t>
+  </si>
+  <si>
+    <t>Peu d'avancée…</t>
+  </si>
+  <si>
+    <t>Total 13.mai</t>
   </si>
 </sst>
 </file>
@@ -928,7 +943,7 @@
   <dimension ref="B2:Z16"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1383,17 +1398,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1405,7 +1420,7 @@
   <dimension ref="B1:X15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1627,7 +1642,7 @@
       <c r="G7" s="24"/>
       <c r="H7" s="28"/>
       <c r="I7" s="24"/>
-      <c r="J7" s="28"/>
+      <c r="J7" s="24"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
@@ -1680,8 +1695,8 @@
       <c r="F9" s="28"/>
       <c r="G9" s="28"/>
       <c r="H9" s="24"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
       <c r="K9" s="28"/>
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
@@ -1735,7 +1750,7 @@
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="24"/>
-      <c r="J11" s="28"/>
+      <c r="J11" s="24"/>
       <c r="K11" s="28"/>
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
@@ -1762,7 +1777,7 @@
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
-      <c r="J12" s="28"/>
+      <c r="J12" s="24"/>
       <c r="K12" s="28"/>
       <c r="L12" s="28"/>
       <c r="M12" s="28"/>
@@ -1843,7 +1858,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
-      <c r="J15" s="31"/>
+      <c r="J15" s="24"/>
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
       <c r="M15" s="31"/>
@@ -1861,17 +1876,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1880,10 +1895,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2227,6 +2242,43 @@
         <v>49</v>
       </c>
     </row>
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="37">
+        <v>43598</v>
+      </c>
+      <c r="B28" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="34">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="37">
+        <v>43598</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="34">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="34">
+        <f>SUM(C24:C29)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Première version qui marche bien
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
   <si>
     <t>Jour</t>
   </si>
@@ -201,6 +201,18 @@
   </si>
   <si>
     <t>Total 13.mai</t>
+  </si>
+  <si>
+    <t>L'analyse est à mon avis suffisante pour le projet. A voir avec M.Bonvin</t>
+  </si>
+  <si>
+    <t>Implémentation de la télécommande du robot</t>
+  </si>
+  <si>
+    <t>Direction, vitesse/compensation, mode manuel/auto</t>
+  </si>
+  <si>
+    <t>Total 14.mai</t>
   </si>
 </sst>
 </file>
@@ -943,7 +955,7 @@
   <dimension ref="B2:Z16"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1643,7 +1655,7 @@
       <c r="H7" s="28"/>
       <c r="I7" s="24"/>
       <c r="J7" s="24"/>
-      <c r="K7" s="28"/>
+      <c r="K7" s="24"/>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
       <c r="N7" s="28"/>
@@ -1671,7 +1683,7 @@
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
+      <c r="L8" s="24"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
       <c r="O8" s="28"/>
@@ -1698,7 +1710,6 @@
       <c r="I9" s="24"/>
       <c r="J9" s="24"/>
       <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
       <c r="M9" s="28"/>
       <c r="N9" s="28"/>
       <c r="O9" s="29"/>
@@ -1752,7 +1763,7 @@
       <c r="I11" s="24"/>
       <c r="J11" s="24"/>
       <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
+      <c r="L11" s="24"/>
       <c r="M11" s="28"/>
       <c r="N11" s="28"/>
       <c r="O11" s="28"/>
@@ -1779,7 +1790,7 @@
       <c r="I12" s="24"/>
       <c r="J12" s="24"/>
       <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
+      <c r="L12" s="24"/>
       <c r="M12" s="28"/>
       <c r="N12" s="28"/>
       <c r="O12" s="28"/>
@@ -1859,8 +1870,8 @@
       <c r="H15" s="24"/>
       <c r="I15" s="24"/>
       <c r="J15" s="24"/>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
       <c r="M15" s="31"/>
       <c r="N15" s="31"/>
       <c r="O15" s="31"/>
@@ -1895,10 +1906,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2279,6 +2290,54 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="37">
+        <v>43599</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="34">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D31" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="37">
+        <v>43599</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="34">
+        <v>0.125</v>
+      </c>
+      <c r="D32" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="37">
+        <v>43599</v>
+      </c>
+      <c r="B33" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="34">
+        <f>SUM(C31:C33)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Documentation de chaque fonction/classe faite
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="62">
   <si>
     <t>Jour</t>
   </si>
@@ -213,6 +213,15 @@
   </si>
   <si>
     <t>Total 14.mai</t>
+  </si>
+  <si>
+    <t>Recherche d'informations sur les méthodes de scikit-image</t>
+  </si>
+  <si>
+    <t>canny, hough_circle, hough_circle_peaks</t>
+  </si>
+  <si>
+    <t>Total 15.mai</t>
   </si>
 </sst>
 </file>
@@ -272,7 +281,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -508,21 +517,6 @@
       </top>
       <bottom style="medium">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,17 +587,17 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -651,7 +645,7 @@
     <tableColumn id="3" name="Temps" dataDxfId="1"/>
     <tableColumn id="4" name="Commentaire" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -955,7 +949,7 @@
   <dimension ref="B2:Z16"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -970,50 +964,50 @@
       <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="39">
         <v>1</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40">
+      <c r="D3" s="38"/>
+      <c r="E3" s="38">
         <v>2</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40">
+      <c r="F3" s="38"/>
+      <c r="G3" s="38">
         <v>3</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40">
+      <c r="H3" s="38"/>
+      <c r="I3" s="38">
         <v>4</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40">
+      <c r="J3" s="38"/>
+      <c r="K3" s="38">
         <v>5</v>
       </c>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40">
+      <c r="L3" s="38"/>
+      <c r="M3" s="38">
         <v>6</v>
       </c>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40">
+      <c r="N3" s="38"/>
+      <c r="O3" s="38">
         <v>7</v>
       </c>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40">
+      <c r="P3" s="38"/>
+      <c r="Q3" s="38">
         <v>8</v>
       </c>
-      <c r="R3" s="40"/>
-      <c r="S3" s="40">
+      <c r="R3" s="38"/>
+      <c r="S3" s="38">
         <v>9</v>
       </c>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40">
+      <c r="T3" s="38"/>
+      <c r="U3" s="38">
         <v>10</v>
       </c>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40">
+      <c r="V3" s="38"/>
+      <c r="W3" s="38">
         <v>11</v>
       </c>
-      <c r="X3" s="40"/>
+      <c r="X3" s="38"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
@@ -1410,17 +1404,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1432,7 +1426,7 @@
   <dimension ref="B1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA12" sqref="AA12"/>
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1446,50 +1440,50 @@
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="39">
         <v>1</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38">
         <v>2</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40">
+      <c r="F2" s="38"/>
+      <c r="G2" s="38">
         <v>3</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40">
+      <c r="H2" s="38"/>
+      <c r="I2" s="38">
         <v>4</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40">
+      <c r="J2" s="38"/>
+      <c r="K2" s="38">
         <v>5</v>
       </c>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40">
+      <c r="L2" s="38"/>
+      <c r="M2" s="38">
         <v>6</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40">
+      <c r="N2" s="38"/>
+      <c r="O2" s="38">
         <v>7</v>
       </c>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40">
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38">
         <v>8</v>
       </c>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40">
+      <c r="R2" s="38"/>
+      <c r="S2" s="38">
         <v>9</v>
       </c>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40">
+      <c r="T2" s="38"/>
+      <c r="U2" s="38">
         <v>10</v>
       </c>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40">
+      <c r="V2" s="38"/>
+      <c r="W2" s="38">
         <v>11</v>
       </c>
-      <c r="X2" s="40"/>
+      <c r="X2" s="38"/>
     </row>
     <row r="3" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
@@ -1679,7 +1673,7 @@
       <c r="E8" s="28"/>
       <c r="F8" s="28"/>
       <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="28"/>
       <c r="J8" s="28"/>
       <c r="K8" s="28"/>
@@ -1764,7 +1758,7 @@
       <c r="J11" s="24"/>
       <c r="K11" s="28"/>
       <c r="L11" s="24"/>
-      <c r="M11" s="28"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="28"/>
       <c r="O11" s="28"/>
       <c r="P11" s="28"/>
@@ -1791,8 +1785,8 @@
       <c r="J12" s="24"/>
       <c r="K12" s="28"/>
       <c r="L12" s="24"/>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
       <c r="O12" s="28"/>
       <c r="P12" s="28"/>
       <c r="Q12" s="28"/>
@@ -1872,8 +1866,8 @@
       <c r="J15" s="24"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
-      <c r="M15" s="31"/>
-      <c r="N15" s="31"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
       <c r="O15" s="31"/>
       <c r="P15" s="31"/>
       <c r="Q15" s="31"/>
@@ -1887,17 +1881,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1906,22 +1900,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.77734375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="34.5546875" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" style="35"/>
-    <col min="4" max="4" width="62.6640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="33"/>
+    <col min="1" max="1" width="8.77734375" style="33"/>
+    <col min="2" max="2" width="26.44140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" style="35"/>
+    <col min="4" max="4" width="59.21875" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.77734375" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>14</v>
       </c>
@@ -1936,101 +1930,101 @@
       </c>
       <c r="K1" s="36"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37">
         <v>43592</v>
       </c>
       <c r="B2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="38">
+      <c r="C2" s="40">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37">
         <v>43592</v>
       </c>
       <c r="B3" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="41">
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="37">
         <v>43592</v>
       </c>
       <c r="B4" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="38">
+      <c r="C4" s="40">
         <v>2.0833333333333332E-2</v>
       </c>
       <c r="D4" s="33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="37">
         <v>43592</v>
       </c>
       <c r="B5" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="41">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="37">
         <v>43592</v>
       </c>
       <c r="B6" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="40">
         <v>6.25E-2</v>
       </c>
       <c r="D6" s="33" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="37">
         <v>43592</v>
       </c>
       <c r="B7" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="39">
+      <c r="C7" s="41">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="37">
         <v>43592</v>
       </c>
       <c r="B8" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="40">
         <v>6.25E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37">
         <v>43592</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="41">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="37">
         <v>43592</v>
       </c>
@@ -2044,7 +2038,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="37"/>
       <c r="B11" s="33" t="s">
         <v>26</v>
@@ -2054,7 +2048,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="37">
         <v>43593</v>
       </c>
@@ -2068,7 +2062,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="37">
         <v>43593</v>
       </c>
@@ -2082,7 +2076,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37">
         <v>43593</v>
       </c>
@@ -2093,7 +2087,7 @@
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="37">
         <v>43593</v>
       </c>
@@ -2107,7 +2101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="37">
         <v>43593</v>
       </c>
@@ -2121,7 +2115,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="33" t="s">
         <v>36</v>
       </c>
@@ -2130,7 +2124,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="37">
         <v>43594</v>
       </c>
@@ -2144,7 +2138,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37">
         <v>43594</v>
       </c>
@@ -2158,7 +2152,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37">
         <v>43594</v>
       </c>
@@ -2169,7 +2163,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37">
         <v>43594</v>
       </c>
@@ -2180,7 +2174,7 @@
         <v>0.10416666666666667</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37">
         <v>43594</v>
       </c>
@@ -2191,7 +2185,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="33" t="s">
         <v>43</v>
       </c>
@@ -2200,7 +2194,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="37">
         <v>43598</v>
       </c>
@@ -2214,7 +2208,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37">
         <v>43598</v>
       </c>
@@ -2228,7 +2222,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37">
         <v>43598</v>
       </c>
@@ -2239,7 +2233,7 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37">
         <v>43598</v>
       </c>
@@ -2253,7 +2247,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37">
         <v>43598</v>
       </c>
@@ -2267,7 +2261,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37">
         <v>43598</v>
       </c>
@@ -2281,7 +2275,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="33" t="s">
         <v>54</v>
       </c>
@@ -2290,7 +2284,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37">
         <v>43599</v>
       </c>
@@ -2304,7 +2298,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="37">
         <v>43599</v>
       </c>
@@ -2318,7 +2312,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="37">
         <v>43599</v>
       </c>
@@ -2329,12 +2323,46 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="33" t="s">
         <v>58</v>
       </c>
       <c r="C34" s="34">
         <f>SUM(C31:C33)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="37">
+        <v>43600</v>
+      </c>
+      <c r="B35" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="34">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D35" s="33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="37">
+        <v>43600</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="34">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="34">
+        <f>SUM(C35:C36)</f>
         <v>0.33333333333333331</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mise à jour rapport de tests et documentations
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>Jour</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t>Total 15.mai</t>
+  </si>
+  <si>
+    <t>Total 16.mai</t>
+  </si>
+  <si>
+    <t>Mise au propre des différents diagrammes</t>
+  </si>
+  <si>
+    <t>Plan et rapport des tests</t>
   </si>
 </sst>
 </file>
@@ -949,7 +958,7 @@
   <dimension ref="B2:Z16"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="AB11" sqref="AB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1404,17 +1413,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1425,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1881,17 +1890,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1900,10 +1909,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2388,6 +2397,48 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
+    <row r="40" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="34">
+        <f>SUM(C38:C39)</f>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="37">
+        <v>43605</v>
+      </c>
+      <c r="B41" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="34">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="37">
+        <v>43605</v>
+      </c>
+      <c r="B42" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="37">
+        <v>43605</v>
+      </c>
+      <c r="B43" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="34">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Beep lorsque balle trouvé Documentations sur les dimensions temporelles
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
   <si>
     <t>Jour</t>
   </si>
@@ -231,13 +231,35 @@
   </si>
   <si>
     <t>Plan et rapport des tests</t>
+  </si>
+  <si>
+    <t>Relecture grille d'évaluation</t>
+  </si>
+  <si>
+    <t>Beep lorsque le robot est proche de la balle</t>
+  </si>
+  <si>
+    <t>Extraction des commentaires docstring en html</t>
+  </si>
+  <si>
+    <t>Total 20.mai</t>
+  </si>
+  <si>
+    <t>Explication des dimensions temporelles</t>
+  </si>
+  <si>
+    <t>Pas réussi - A revoir</t>
+  </si>
+  <si>
+    <t>Questions / Réponses
+Remarque sur les tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +269,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -533,7 +563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -602,6 +632,15 @@
     <xf numFmtId="20" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -646,8 +685,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D53" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D53"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D60" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D60"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Date" dataDxfId="3"/>
     <tableColumn id="2" name="Tâche" dataDxfId="2"/>
@@ -958,7 +997,7 @@
   <dimension ref="B2:Z16"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,50 +1012,50 @@
       <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="41">
+      <c r="C3" s="44">
         <v>1</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43">
         <v>2</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40">
+      <c r="F3" s="43"/>
+      <c r="G3" s="43">
         <v>3</v>
       </c>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40">
+      <c r="H3" s="43"/>
+      <c r="I3" s="43">
         <v>4</v>
       </c>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40">
+      <c r="J3" s="43"/>
+      <c r="K3" s="43">
         <v>5</v>
       </c>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40">
+      <c r="L3" s="43"/>
+      <c r="M3" s="43">
         <v>6</v>
       </c>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40">
+      <c r="N3" s="43"/>
+      <c r="O3" s="43">
         <v>7</v>
       </c>
-      <c r="P3" s="40"/>
-      <c r="Q3" s="40">
+      <c r="P3" s="43"/>
+      <c r="Q3" s="43">
         <v>8</v>
       </c>
-      <c r="R3" s="40"/>
-      <c r="S3" s="40">
+      <c r="R3" s="43"/>
+      <c r="S3" s="43">
         <v>9</v>
       </c>
-      <c r="T3" s="40"/>
-      <c r="U3" s="40">
+      <c r="T3" s="43"/>
+      <c r="U3" s="43">
         <v>10</v>
       </c>
-      <c r="V3" s="40"/>
-      <c r="W3" s="40">
+      <c r="V3" s="43"/>
+      <c r="W3" s="43">
         <v>11</v>
       </c>
-      <c r="X3" s="40"/>
+      <c r="X3" s="43"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
     </row>
@@ -1413,17 +1452,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1435,7 +1474,7 @@
   <dimension ref="B1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1449,50 +1488,50 @@
       <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41">
+      <c r="C2" s="44">
         <v>1</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40">
+      <c r="D2" s="43"/>
+      <c r="E2" s="43">
         <v>2</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40">
+      <c r="F2" s="43"/>
+      <c r="G2" s="43">
         <v>3</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40">
+      <c r="H2" s="43"/>
+      <c r="I2" s="43">
         <v>4</v>
       </c>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40">
+      <c r="J2" s="43"/>
+      <c r="K2" s="43">
         <v>5</v>
       </c>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40">
+      <c r="L2" s="43"/>
+      <c r="M2" s="43">
         <v>6</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40">
+      <c r="N2" s="43"/>
+      <c r="O2" s="43">
         <v>7</v>
       </c>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40">
+      <c r="P2" s="43"/>
+      <c r="Q2" s="43">
         <v>8</v>
       </c>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40">
+      <c r="R2" s="43"/>
+      <c r="S2" s="43">
         <v>9</v>
       </c>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40">
+      <c r="T2" s="43"/>
+      <c r="U2" s="43">
         <v>10</v>
       </c>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40">
+      <c r="V2" s="43"/>
+      <c r="W2" s="43">
         <v>11</v>
       </c>
-      <c r="X2" s="40"/>
+      <c r="X2" s="43"/>
     </row>
     <row r="3" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
@@ -1717,8 +1756,8 @@
       <c r="N9" s="28"/>
       <c r="O9" s="29"/>
       <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="24"/>
       <c r="S9" s="28"/>
       <c r="T9" s="28"/>
       <c r="U9" s="28"/>
@@ -1744,7 +1783,6 @@
       <c r="N10" s="28"/>
       <c r="O10" s="28"/>
       <c r="P10" s="28"/>
-      <c r="Q10" s="29"/>
       <c r="R10" s="28"/>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
@@ -1772,8 +1810,8 @@
       <c r="O11" s="28"/>
       <c r="P11" s="28"/>
       <c r="Q11" s="24"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="28"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
       <c r="T11" s="28"/>
       <c r="U11" s="28"/>
       <c r="V11" s="28"/>
@@ -1799,8 +1837,8 @@
       <c r="O12" s="24"/>
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
-      <c r="R12" s="28"/>
-      <c r="S12" s="28"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
       <c r="T12" s="28"/>
       <c r="U12" s="28"/>
       <c r="V12" s="28"/>
@@ -1880,8 +1918,8 @@
       <c r="O15" s="24"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
-      <c r="R15" s="31"/>
-      <c r="S15" s="31"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
       <c r="T15" s="31"/>
       <c r="U15" s="31"/>
       <c r="V15" s="31"/>
@@ -1890,17 +1928,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1909,10 +1947,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2047,12 +2085,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
-      <c r="B11" s="33" t="s">
+    <row r="11" spans="1:11" s="40" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="42"/>
+      <c r="B11" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="34">
+      <c r="C11" s="41">
         <f>SUM(C2:C10)</f>
         <v>0.33333333333333337</v>
       </c>
@@ -2124,11 +2162,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="33" t="s">
+    <row r="17" spans="1:4" s="40" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="34">
+      <c r="C17" s="41">
         <f>SUM(C12:C16)</f>
         <v>0.33333333333333331</v>
       </c>
@@ -2194,11 +2232,11 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="33" t="s">
+    <row r="23" spans="1:4" s="40" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="41">
         <f>SUM(C18:C22)</f>
         <v>0.33333333333333337</v>
       </c>
@@ -2284,11 +2322,11 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="33" t="s">
+    <row r="30" spans="1:4" s="40" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="34">
+      <c r="C30" s="41">
         <f>SUM(C24:C29)</f>
         <v>0.33333333333333331</v>
       </c>
@@ -2332,11 +2370,11 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="33" t="s">
+    <row r="34" spans="1:4" s="40" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="34">
+      <c r="C34" s="41">
         <f>SUM(C31:C33)</f>
         <v>0.33333333333333331</v>
       </c>
@@ -2366,11 +2404,11 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="33" t="s">
+    <row r="37" spans="1:4" s="40" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="34">
+      <c r="C37" s="41">
         <f>SUM(C35:C36)</f>
         <v>0.33333333333333331</v>
       </c>
@@ -2397,11 +2435,11 @@
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="33" t="s">
+    <row r="40" spans="1:4" s="40" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="34">
+      <c r="C40" s="41">
         <f>SUM(C38:C39)</f>
         <v>0.33333333333333331</v>
       </c>
@@ -2437,6 +2475,79 @@
       </c>
       <c r="C43" s="34">
         <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="37">
+        <v>43605</v>
+      </c>
+      <c r="B44" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="37">
+        <v>43605</v>
+      </c>
+      <c r="B45" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="34">
+        <v>2.0833333333333332E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="37">
+        <v>43605</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="34">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D46" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="37">
+        <v>43605</v>
+      </c>
+      <c r="B47" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="34">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="C48" s="34">
+        <f>SUM(C41:C47)</f>
+        <v>0.35416666666666663</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="37">
+        <v>43606</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="34">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Protocle de tests Documentation
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
   <si>
     <t>Jour</t>
   </si>
@@ -253,6 +253,15 @@
   <si>
     <t>Questions / Réponses
 Remarque sur les tests</t>
+  </si>
+  <si>
+    <t>Protocole de tests</t>
+  </si>
+  <si>
+    <t>Création d'une image avec les librairies utiles au programme</t>
+  </si>
+  <si>
+    <t>Total 21.mai</t>
   </si>
 </sst>
 </file>
@@ -1452,17 +1461,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1474,7 +1483,7 @@
   <dimension ref="B1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1812,7 +1821,7 @@
       <c r="Q11" s="24"/>
       <c r="R11" s="24"/>
       <c r="S11" s="24"/>
-      <c r="T11" s="28"/>
+      <c r="T11" s="24"/>
       <c r="U11" s="28"/>
       <c r="V11" s="28"/>
       <c r="W11" s="28"/>
@@ -1839,7 +1848,7 @@
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
       <c r="S12" s="24"/>
-      <c r="T12" s="28"/>
+      <c r="T12" s="24"/>
       <c r="U12" s="28"/>
       <c r="V12" s="28"/>
       <c r="W12" s="28"/>
@@ -1920,7 +1929,7 @@
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="31"/>
+      <c r="T15" s="24"/>
       <c r="U15" s="31"/>
       <c r="V15" s="31"/>
       <c r="W15" s="31"/>
@@ -1928,17 +1937,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="W2:X2"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1947,10 +1956,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2531,7 +2540,7 @@
       <c r="B48" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C48" s="34">
+      <c r="C48" s="41">
         <f>SUM(C41:C47)</f>
         <v>0.35416666666666663</v>
       </c>
@@ -2544,10 +2553,38 @@
         <v>6</v>
       </c>
       <c r="C49" s="34">
-        <v>0.16666666666666666</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="D49" s="33" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C51" s="34">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D51" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="40" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="C52" s="41">
+        <f>SUM(C49:C51)</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalisation protocoles de tests Réduction de la résolution de caméra Résumé du rapport Documentaion
</commit_message>
<xml_diff>
--- a/Documents/Planning_TPI_Forestier.xlsx
+++ b/Documents/Planning_TPI_Forestier.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8616"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionel" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Jour</t>
   </si>
@@ -262,6 +262,21 @@
   </si>
   <si>
     <t>Total 21.mai</t>
+  </si>
+  <si>
+    <t>Manque le fichier robot_controller.py car ce n'est pas une classe</t>
+  </si>
+  <si>
+    <t>Visite des M.Bonvin</t>
+  </si>
+  <si>
+    <t>création d'une image livrable pour le projet</t>
+  </si>
+  <si>
+    <t>Total 22.mai</t>
+  </si>
+  <si>
+    <t>Résumé du rapport</t>
   </si>
 </sst>
 </file>
@@ -694,8 +709,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D60" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:D63" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D63"/>
   <tableColumns count="4">
     <tableColumn id="1" name="Date" dataDxfId="3"/>
     <tableColumn id="2" name="Tâche" dataDxfId="2"/>
@@ -1005,8 +1020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Z16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1482,8 +1497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V13" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1795,8 +1810,8 @@
       <c r="R10" s="28"/>
       <c r="S10" s="28"/>
       <c r="T10" s="28"/>
-      <c r="U10" s="28"/>
-      <c r="V10" s="28"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
       <c r="W10" s="28"/>
       <c r="X10" s="30"/>
     </row>
@@ -1822,7 +1837,7 @@
       <c r="R11" s="24"/>
       <c r="S11" s="24"/>
       <c r="T11" s="24"/>
-      <c r="U11" s="28"/>
+      <c r="U11" s="24"/>
       <c r="V11" s="28"/>
       <c r="W11" s="28"/>
       <c r="X11" s="30"/>
@@ -1849,8 +1864,8 @@
       <c r="R12" s="24"/>
       <c r="S12" s="24"/>
       <c r="T12" s="24"/>
-      <c r="U12" s="28"/>
-      <c r="V12" s="28"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
       <c r="W12" s="28"/>
       <c r="X12" s="30"/>
     </row>
@@ -1877,7 +1892,7 @@
       <c r="S13" s="28"/>
       <c r="T13" s="28"/>
       <c r="U13" s="28"/>
-      <c r="V13" s="29"/>
+      <c r="V13" s="24"/>
       <c r="W13" s="28"/>
       <c r="X13" s="30"/>
     </row>
@@ -1930,8 +1945,8 @@
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
       <c r="T15" s="24"/>
-      <c r="U15" s="31"/>
-      <c r="V15" s="31"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
       <c r="W15" s="31"/>
       <c r="X15" s="32"/>
     </row>
@@ -1956,10 +1971,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K52"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="36.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2587,6 +2602,79 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
+    <row r="53" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="37">
+        <v>43607</v>
+      </c>
+      <c r="B53" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D53" s="33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="37">
+        <v>43607</v>
+      </c>
+      <c r="B54" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="34">
+        <v>0.14583333333333334</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="37">
+        <v>43607</v>
+      </c>
+      <c r="B55" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="37">
+        <v>43607</v>
+      </c>
+      <c r="B56" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="34">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D56" s="33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="40" customFormat="1" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="37">
+        <v>43607</v>
+      </c>
+      <c r="B57" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="34">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D57" s="33"/>
+    </row>
+    <row r="58" spans="1:4" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="40"/>
+      <c r="B58" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C58" s="41">
+        <f>SUM(C53:C57)</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D58" s="40"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>